<commit_message>
updated tank and controller assembly
</commit_message>
<xml_diff>
--- a/Materials/CBASS_Parts_List.xlsx
+++ b/Materials/CBASS_Parts_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2917054de0bc48a0/Documents/Barshis_Lab/BarshisLab_Github/CBASS_Manual/Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6A953C9003A2749FC107CC9D4D61295D6BD9AC6C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3C64105-6635-4D5C-8C66-D7171C917982}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_6A953C9003A2749FC107CC9D4D61295D6BD9AC6C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49B36079-43C6-42C6-B8E5-89BB060082FF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -930,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1243,7 +1243,7 @@
       <c r="E8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="37" t="s">
         <v>23</v>
       </c>
       <c r="G8" s="10"/>
@@ -29649,6 +29649,7 @@
     <hyperlink ref="F62" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
     <hyperlink ref="F29" r:id="rId29" xr:uid="{6B2C8CED-3408-4A95-9E5E-893891A37281}"/>
     <hyperlink ref="F4" r:id="rId30" xr:uid="{78E454CC-EFC9-4B18-81B6-BE01FE6120B7}"/>
+    <hyperlink ref="F8" r:id="rId31" xr:uid="{6DAB66AF-D7A0-46A0-8997-CC26311CA373}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>